<commit_message>
update data excel end change color border zoning
</commit_message>
<xml_diff>
--- a/public/template_excel.xlsx
+++ b/public/template_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asnur\Documents\Kantor\sip-dev-laravel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E0D5AE-5233-4D84-A7EE-DF9EAC22A159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6449DB-E539-4A8C-8C15-526444365031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0130DBD8-6A69-4CBA-912A-B552F28C542C}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I2" sqref="I2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,7 +790,7 @@
       <formula1>"TP-1,TP-2,TP-2.1,TP-2.2,TP-3,TP-4,TP-5,TP-6,KK,BP,RP"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6" xr:uid="{D38EC2FD-919E-4203-BA1E-C087F3617E9E}">
-      <formula1>"-,LP-C,LP-M,LP-KR,LP-CR,LP-MR,LK"</formula1>
+      <formula1>"-,LP-C,LP-M,LP-KR,LP-CR,LP-MR,LK,LP-K"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{BD881627-4478-40AA-8A09-F63FA1899F88}">
       <formula1>"PL,PB-1,PB-2,PB-3,PB-4"</formula1>

</xml_diff>

<commit_message>
update input with global_id
</commit_message>
<xml_diff>
--- a/public/template_excel.xlsx
+++ b/public/template_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asnur\Documents\Kantor\sip-dev-laravel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6449DB-E539-4A8C-8C15-526444365031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE960E0C-D965-4A46-A050-EDFC269381B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0130DBD8-6A69-4CBA-912A-B552F28C542C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Warteg Bahari Baruasd</t>
   </si>
@@ -159,6 +159,24 @@
   </si>
   <si>
     <t>Koordinat</t>
+  </si>
+  <si>
+    <t>Global ID</t>
+  </si>
+  <si>
+    <t>{12BCC37E-15D7-4AA5-9287-7FBEE2C31483}</t>
+  </si>
+  <si>
+    <t>{12BCC37E-15D7-IJNLKA-9287-ASDAS080122}</t>
+  </si>
+  <si>
+    <t>{12BCC37E-15D7-ASDS-9287-POP21389123}</t>
+  </si>
+  <si>
+    <t>{12BCC37E-15D7-4AA5-9287-ASDASD1389183}</t>
+  </si>
+  <si>
+    <t>{12BCC37E-15D7-4AA5-9287-ASKPQ09121133}</t>
   </si>
 </sst>
 </file>
@@ -529,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FBF871-B1EA-449D-87AB-E25E2A06AEC1}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I6"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,9 +566,10 @@
     <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -587,8 +606,11 @@
       <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="str">
         <f>RIGHT(LEFT(C2,SEARCH(",",C2,1)-1),4)&amp;RIGHT(RIGHT(C2,SEARCH(",",C2,1)-1),4)</f>
         <v>87089973</v>
@@ -626,8 +648,11 @@
       <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="str">
         <f t="shared" ref="A3" si="0">RIGHT(LEFT(C3,SEARCH(",",C3,1)-1),4)&amp;RIGHT(RIGHT(C3,SEARCH(",",C3,1)-1),4)</f>
         <v>41106135</v>
@@ -665,8 +690,11 @@
       <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="M3" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="str">
         <f t="shared" ref="A4:A6" si="1">RIGHT(LEFT(C4,SEARCH(",",C4,1)-1),4)&amp;RIGHT(RIGHT(C4,SEARCH(",",C4,1)-1),4)</f>
         <v>91960372</v>
@@ -704,8 +732,11 @@
       <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
         <v>00861177</v>
@@ -743,8 +774,11 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="M5" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
         <v>56115202</v>
@@ -781,6 +815,9 @@
       </c>
       <c r="L6" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -800,5 +837,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>